<commit_message>
Signed-off-by: Alem Luckin <aluckin2@etf.unsa.ba>
</commit_message>
<xml_diff>
--- a/UseCaseScenarij/Registracija Objekta.xlsx
+++ b/UseCaseScenarij/Registracija Objekta.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alem\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alem\KlixNightlife\UseCaseScenarij\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -80,9 +80,6 @@
     <t>1. Pristupa interfejsu za registraciju</t>
   </si>
   <si>
-    <t>2. Popunjava licne podatke i podatke u vezi objekta</t>
-  </si>
-  <si>
     <t>3.Salje zahtjev za registraciju</t>
   </si>
   <si>
@@ -114,6 +111,9 @@
   </si>
   <si>
     <t>7. Salje potvrdni mail korisniku</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2. Popunjava licne podatke </t>
   </si>
 </sst>
 </file>
@@ -522,8 +522,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="B24" sqref="B24"/>
+    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -592,7 +592,7 @@
     </row>
     <row r="8" spans="1:3" ht="87" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="8" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B8" s="6"/>
       <c r="C8" s="7"/>
@@ -615,16 +615,16 @@
       <c r="B10" s="2"/>
       <c r="C10" s="2"/>
     </row>
-    <row r="11" spans="1:3" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
-        <v>18</v>
+        <v>29</v>
       </c>
       <c r="B11" s="2"/>
       <c r="C11" s="2"/>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B12" s="2"/>
       <c r="C12" s="2"/>
@@ -632,7 +632,7 @@
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="2"/>
       <c r="B13" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C13" s="2"/>
     </row>
@@ -640,20 +640,20 @@
       <c r="A14" s="2"/>
       <c r="B14" s="2"/>
       <c r="C14" s="4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="15" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="2"/>
       <c r="B15" s="2"/>
       <c r="C15" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="16" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="2"/>
       <c r="B16" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C16" s="4"/>
     </row>
@@ -664,10 +664,10 @@
     </row>
     <row r="18" spans="1:3" ht="118.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="B18" s="13" t="s">
         <v>23</v>
-      </c>
-      <c r="B18" s="13" t="s">
-        <v>24</v>
       </c>
       <c r="C18" s="14"/>
     </row>
@@ -686,20 +686,20 @@
       <c r="A20" s="9"/>
       <c r="B20" s="9"/>
       <c r="C20" s="10" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="21" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="2"/>
       <c r="B21" s="2"/>
       <c r="C21" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="2"/>
       <c r="B22" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C22" s="2"/>
     </row>

</xml_diff>